<commit_message>
Otomatik İşlemler Kümülatif Toplam Sayfalar Arası Toplama Yöntemleri
</commit_message>
<xml_diff>
--- a/working 12.xlsx
+++ b/working 12.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KÜMÜLATİF TOPLAM" sheetId="1" r:id="rId1"/>
     <sheet name="OTOMATİK TOPLAM" sheetId="3" r:id="rId2"/>
+    <sheet name="Sayfalar Arası Formül Kullanımı" sheetId="4" r:id="rId3"/>
+    <sheet name="Ocak" sheetId="5" r:id="rId4"/>
+    <sheet name="Şubat" sheetId="6" r:id="rId5"/>
+    <sheet name="Mart" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Kasadan Harcanan</t>
   </si>
@@ -50,13 +54,49 @@
   </si>
   <si>
     <t>Örnek Toplam</t>
+  </si>
+  <si>
+    <t>OCAK</t>
+  </si>
+  <si>
+    <t>Ürün Adı</t>
+  </si>
+  <si>
+    <t>Satış Adedi</t>
+  </si>
+  <si>
+    <t>Tutar</t>
+  </si>
+  <si>
+    <t>A Ürünü</t>
+  </si>
+  <si>
+    <t>B Ürünü</t>
+  </si>
+  <si>
+    <t>C Ürünü</t>
+  </si>
+  <si>
+    <t>D Ürünü</t>
+  </si>
+  <si>
+    <t>ŞUBAT</t>
+  </si>
+  <si>
+    <t>MART</t>
+  </si>
+  <si>
+    <t>TOPLAM</t>
+  </si>
+  <si>
+    <t>Değiştirildi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +130,24 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +163,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,8 +280,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -217,23 +302,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,35 +613,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>43101</v>
       </c>
       <c r="B3">
@@ -564,19 +651,19 @@
         <f>IF(B3="","",SUM($B$3:B3))</f>
         <v>450</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="2">
         <v>43102</v>
       </c>
       <c r="B4">
@@ -586,17 +673,17 @@
         <f>IF(B4="","",SUM($B$3:B4))</f>
         <v>600</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="2">
         <v>43103</v>
       </c>
       <c r="B5">
@@ -606,17 +693,17 @@
         <f>IF(B5="","",SUM($B$3:B5))</f>
         <v>800</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="2">
         <v>43104</v>
       </c>
       <c r="B6">
@@ -626,17 +713,17 @@
         <f>IF(B6="","",SUM($B$3:B6))</f>
         <v>1050</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="2">
         <v>43105</v>
       </c>
       <c r="B7">
@@ -648,7 +735,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="2">
         <v>43106</v>
       </c>
       <c r="B8">
@@ -660,7 +747,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="2">
         <v>43107</v>
       </c>
       <c r="B9">
@@ -672,7 +759,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="2">
         <v>43108</v>
       </c>
       <c r="B10">
@@ -684,7 +771,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="2">
         <v>43109</v>
       </c>
       <c r="B11">
@@ -696,7 +783,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="2">
         <v>43110</v>
       </c>
       <c r="B12">
@@ -708,7 +795,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="2">
         <v>43111</v>
       </c>
       <c r="B13">
@@ -720,7 +807,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="2">
         <v>43112</v>
       </c>
       <c r="B14">
@@ -732,7 +819,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="2">
         <v>43113</v>
       </c>
       <c r="B15">
@@ -744,7 +831,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="2">
         <v>43114</v>
       </c>
       <c r="B16">
@@ -756,7 +843,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="2">
         <v>43115</v>
       </c>
       <c r="B17">
@@ -768,7 +855,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="2">
         <v>43116</v>
       </c>
       <c r="B18">
@@ -780,7 +867,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="2">
         <v>43117</v>
       </c>
       <c r="B19">
@@ -792,7 +879,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="2">
         <v>43118</v>
       </c>
       <c r="C20" t="str">
@@ -801,7 +888,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="A21" s="2">
         <v>43119</v>
       </c>
       <c r="C21" t="str">
@@ -810,7 +897,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="A22" s="2">
         <v>43120</v>
       </c>
       <c r="C22" t="str">
@@ -819,7 +906,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="A23" s="2">
         <v>43121</v>
       </c>
       <c r="B23">
@@ -831,7 +918,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="A24" s="2">
         <v>43122</v>
       </c>
       <c r="C24" t="str">
@@ -840,7 +927,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+      <c r="A25" s="2">
         <v>43123</v>
       </c>
       <c r="C25" t="str">
@@ -849,7 +936,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="A26" s="2">
         <v>43124</v>
       </c>
       <c r="C26" t="str">
@@ -858,7 +945,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+      <c r="A27" s="2">
         <v>43125</v>
       </c>
       <c r="C27" t="str">
@@ -867,7 +954,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="A28" s="2">
         <v>43126</v>
       </c>
       <c r="C28" t="str">
@@ -876,7 +963,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="2">
         <v>43127</v>
       </c>
       <c r="C29" t="str">
@@ -885,7 +972,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="A30" s="2">
         <v>43128</v>
       </c>
       <c r="C30" t="str">
@@ -894,7 +981,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="2">
         <v>43129</v>
       </c>
       <c r="C31" t="str">
@@ -903,7 +990,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+      <c r="A32" s="2">
         <v>43130</v>
       </c>
       <c r="C32" t="str">
@@ -912,7 +999,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="A33" s="2">
         <v>43131</v>
       </c>
       <c r="C33" t="str">
@@ -921,7 +1008,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+      <c r="A34" s="2">
         <v>43132</v>
       </c>
       <c r="C34" t="str">
@@ -930,7 +1017,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="A35" s="2">
         <v>43133</v>
       </c>
       <c r="C35" t="str">
@@ -959,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -969,35 +1056,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="2">
         <v>43101</v>
       </c>
       <c r="B3">
@@ -1018,7 +1105,7 @@
       <c r="L3" s="10"/>
     </row>
     <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="2">
         <v>43102</v>
       </c>
       <c r="B4">
@@ -1037,7 +1124,7 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="2">
         <v>43103</v>
       </c>
       <c r="B5">
@@ -1056,7 +1143,7 @@
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="2">
         <v>43104</v>
       </c>
       <c r="B6">
@@ -1075,7 +1162,7 @@
       <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="2">
         <v>43105</v>
       </c>
       <c r="B7">
@@ -1086,7 +1173,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="2">
         <v>43106</v>
       </c>
       <c r="B8">
@@ -1097,7 +1184,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="2">
         <v>43107</v>
       </c>
       <c r="B9">
@@ -1129,7 +1216,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="2">
         <v>43108</v>
       </c>
       <c r="B10">
@@ -1140,7 +1227,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="2">
         <v>43109</v>
       </c>
       <c r="B11">
@@ -1151,7 +1238,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="2">
         <v>43110</v>
       </c>
       <c r="B12">
@@ -1162,7 +1249,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="2">
         <v>43111</v>
       </c>
       <c r="B13">
@@ -1173,7 +1260,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="2">
         <v>43112</v>
       </c>
       <c r="B14">
@@ -1184,7 +1271,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="2">
         <v>43113</v>
       </c>
       <c r="B15">
@@ -1195,7 +1282,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="2">
         <v>43114</v>
       </c>
       <c r="B16">
@@ -1206,7 +1293,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+      <c r="A17" s="2">
         <v>43115</v>
       </c>
       <c r="B17">
@@ -1217,7 +1304,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="2">
         <v>43116</v>
       </c>
       <c r="B18">
@@ -1228,7 +1315,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="2">
         <v>43117</v>
       </c>
       <c r="B19">
@@ -1239,7 +1326,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="2">
         <v>43118</v>
       </c>
       <c r="B20">
@@ -1250,7 +1337,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="A21" s="2">
         <v>43119</v>
       </c>
       <c r="B21">
@@ -1261,7 +1348,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="A22" s="2">
         <v>43120</v>
       </c>
       <c r="B22">
@@ -1272,7 +1359,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="A23" s="2">
         <v>43121</v>
       </c>
       <c r="B23">
@@ -1283,7 +1370,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="A24" s="2">
         <v>43122</v>
       </c>
       <c r="B24">
@@ -1296,7 +1383,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+      <c r="A25" s="2">
         <v>43123</v>
       </c>
       <c r="B25">
@@ -1309,7 +1396,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="A26" s="2">
         <v>43124</v>
       </c>
       <c r="B26">
@@ -1322,7 +1409,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="9">
+      <c r="A27" s="2">
         <v>43125</v>
       </c>
       <c r="B27">
@@ -1335,7 +1422,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="A28" s="2">
         <v>43126</v>
       </c>
       <c r="B28">
@@ -1348,37 +1435,37 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="2">
         <v>43127</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="9">
+      <c r="A30" s="2">
         <v>43128</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="9">
+      <c r="A31" s="2">
         <v>43129</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="9">
+      <c r="A32" s="2">
         <v>43130</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="A33" s="2">
         <v>43131</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
+      <c r="A34" s="2">
         <v>43132</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="A35" s="2">
         <v>43133</v>
       </c>
     </row>
@@ -1391,4 +1478,412 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" t="str">
+        <f>Ocak!F4</f>
+        <v>Değiştirildi</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <f>Ocak!B3+Şubat!B3+Mart!B3</f>
+        <v>58</v>
+      </c>
+      <c r="C3">
+        <f>Ocak!C3+Şubat!C3+Mart!C3</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
+        <f>Ocak!B4+Şubat!B4+Mart!B4</f>
+        <v>116</v>
+      </c>
+      <c r="C4" s="15">
+        <f>Ocak!C4+Şubat!C4+Mart!C4</f>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f>SUM(Ocak!B5,Şubat!B5,Mart!B5)</f>
+        <v>174</v>
+      </c>
+      <c r="C5">
+        <f>SUM(Ocak!C5,Şubat!C5,Mart!C5)</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15">
+        <f>SUM(Ocak!B6,Şubat!B6,Mart!B6)</f>
+        <v>232</v>
+      </c>
+      <c r="C6" s="15">
+        <f>SUM(Ocak!C6,Şubat!C6,Mart!C6)</f>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f>SUM(Ocak!B7,Şubat!B7,Mart!B7)</f>
+        <v>580</v>
+      </c>
+      <c r="C7">
+        <f>SUM(Ocak!C7,Şubat!C7,Mart!C7)</f>
+        <v>3300</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10</v>
+      </c>
+      <c r="C4" s="15">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B3:B6)</f>
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15">
+        <v>12</v>
+      </c>
+      <c r="C6" s="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B3:B6)</f>
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
+        <v>100</v>
+      </c>
+      <c r="C4" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15">
+        <v>200</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B3:B6)</f>
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C3:C6)</f>
+        <v>2500</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>